<commit_message>
interpolation and eda newdata
</commit_message>
<xml_diff>
--- a/Teamwork/quarterly_data.xlsx
+++ b/Teamwork/quarterly_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Desktop\2023.1\ATS\BaiTapNhom\ATS\Teamwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB96643-2734-4353-94E3-4D0CAE7A41AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89175E1E-314C-4EF5-B32D-CD94E2BFC6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,12 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -150,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -160,6 +166,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -495,70 +505,70 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>5403820</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>3549378.3664637278</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>10635856</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>8224063.9397626687</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>13296226</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>7190059.0101799984</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>10013404</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>6146164.0311200004</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>